<commit_message>
get Companies route mod
</commit_message>
<xml_diff>
--- a/Книга1.xlsx
+++ b/Книга1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mtseng\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mtseng\Desktop\express\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAFD4B7-099B-40F9-9331-EE81ACE64732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07E3F91-DB1E-42B5-A415-E11ADA65D269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F55CFF5A-F216-469B-BBF9-21BB09FB9AA5}"/>
   </bookViews>
@@ -169,9 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -489,7 +490,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,7 +534,7 @@
       <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>SUM(E3:E6)</f>
         <v>172565</v>
       </c>
@@ -554,7 +555,7 @@
       <c r="D3">
         <v>101</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>151917</v>
       </c>
       <c r="F3">
@@ -574,7 +575,7 @@
       <c r="D4">
         <v>102</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>2382</v>
       </c>
       <c r="F4">
@@ -594,7 +595,7 @@
       <c r="D5">
         <v>103</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>15235</v>
       </c>
       <c r="F5">
@@ -614,7 +615,7 @@
       <c r="D6">
         <v>104</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>3031</v>
       </c>
       <c r="F6">
@@ -634,7 +635,7 @@
       <c r="D7">
         <v>105</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>212763</v>
       </c>
       <c r="F7">
@@ -654,7 +655,7 @@
       <c r="D8">
         <v>106</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>146225</v>
       </c>
       <c r="F8">
@@ -674,7 +675,7 @@
       <c r="D9">
         <v>107</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>945</v>
       </c>
       <c r="F9">
@@ -694,7 +695,7 @@
       <c r="D10">
         <v>108</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>38581</v>
       </c>
       <c r="F10">
@@ -714,7 +715,7 @@
       <c r="D11">
         <v>109</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>200</v>
       </c>
       <c r="F11">
@@ -734,7 +735,7 @@
       <c r="D12">
         <v>110</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>26812</v>
       </c>
       <c r="F12">
@@ -754,7 +755,7 @@
       <c r="D13">
         <v>111</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>310939</v>
       </c>
       <c r="F13">
@@ -774,7 +775,7 @@
       <c r="D14">
         <v>112</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>8498</v>
       </c>
       <c r="F14">
@@ -794,7 +795,7 @@
       <c r="D15">
         <v>113</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>21600</v>
       </c>
       <c r="F15">
@@ -814,7 +815,7 @@
       <c r="D16">
         <v>114</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>41459</v>
       </c>
       <c r="F16">
@@ -834,7 +835,7 @@
       <c r="D17">
         <v>115</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>2832</v>
       </c>
       <c r="F17">
@@ -851,7 +852,7 @@
       <c r="D18">
         <v>200</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <f>(E12+E11)/E15</f>
         <v>1.2505555555555556</v>
       </c>
@@ -869,7 +870,7 @@
       <c r="D19">
         <v>201</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <f>(E12+E11+E10)/E15</f>
         <v>3.0367129629629628</v>
       </c>
@@ -887,7 +888,7 @@
       <c r="D20">
         <v>202</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <f>E7/(E16+E15)</f>
         <v>3.3740306696902902</v>
       </c>
@@ -908,7 +909,7 @@
       <c r="D21">
         <v>203</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <f>E7-E15</f>
         <v>191163</v>
       </c>
@@ -926,7 +927,7 @@
       <c r="D22">
         <v>300</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="2">
         <f>E15/E13</f>
         <v>6.9467001566223596E-2</v>
       </c>
@@ -944,7 +945,7 @@
       <c r="D23">
         <v>301</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="2">
         <f>E13/(E2+E7+SUM(E13:E17))</f>
         <v>0.40347314495702363</v>
       </c>
@@ -962,7 +963,7 @@
       <c r="D24">
         <v>302</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <f>E13/E15</f>
         <v>14.395324074074074</v>
       </c>
@@ -980,7 +981,7 @@
       <c r="D25">
         <v>303</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <f>(E13+E14)/(E2+E7+SUM(E13:E17))</f>
         <v>0.41450011418843169</v>
       </c>

</xml_diff>